<commit_message>
perbaikan import dan excel mahasiswa
</commit_message>
<xml_diff>
--- a/public/template_mahasiswa.xlsx
+++ b/public/template_mahasiswa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949B44C8-3F31-48A7-AC1A-218A31D71B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCD181C-BA99-4C9A-AB7A-2A334344F4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>nim</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>id_kategori</t>
   </si>
   <si>
     <t>Alvini kedua</t>
@@ -408,7 +405,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,22 +450,20 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>23415270</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>2023</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>383745324</v>
@@ -484,9 +479,6 @@
       </c>
       <c r="I2">
         <v>1</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update import and update template excel mahasiswa
* navbar baru

* tambah inputan

* ganti icon ni ni

* commit role

* nambah crud admin

* add fitur import mahasiswa,dospem

* perbaikan import dan excel mahasiswa
</commit_message>
<xml_diff>
--- a/public/template_mahasiswa.xlsx
+++ b/public/template_mahasiswa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949B44C8-3F31-48A7-AC1A-218A31D71B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCD181C-BA99-4C9A-AB7A-2A334344F4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>nim</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>id_kategori</t>
   </si>
   <si>
     <t>Alvini kedua</t>
@@ -408,7 +405,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,22 +450,20 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>23415270</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>2023</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>383745324</v>
@@ -484,9 +479,6 @@
       </c>
       <c r="I2">
         <v>1</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>